<commit_message>
date issue in import file fixed.....
</commit_message>
<xml_diff>
--- a/public/guidance-report.xlsx
+++ b/public/guidance-report.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biahmed\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bilal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032A1077-4FE8-46A9-A0BD-76DA40B3D922}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" forceFullCalc="1"/>
+  <calcPr calcId="179021" forceFullCalc="1"/>
 </workbook>
 </file>
 
@@ -57,10 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yyyy;@"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,9 +86,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,7 +183,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,14 +391,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
@@ -415,7 +412,7 @@
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,13 +446,9 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>